<commit_message>
S00034 - Another text extraction bug fix. Who would've guessed woooooooow
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76221029-C909-4195-8B47-2A8717A2CDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51433661-B278-46F8-AFDA-579E51B46D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="11550" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="10140" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3750,7 +3750,7 @@
   <dimension ref="A1:E1108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
-      <selection activeCell="B452" sqref="B452"/>
+      <selection activeCell="D450" sqref="D450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -6059,6 +6059,12 @@
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>451</v>
+      </c>
+      <c r="B452" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C452" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
S10000. Also fix voice on breaks.
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4E1A1-8FF8-4F52-B62A-3DDE98468688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA494F17-4527-4540-8353-601BD09C4B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="11190" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="8640" windowWidth="53505" windowHeight="21495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3750,7 +3750,7 @@
   <dimension ref="A1:E1108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
-      <selection activeCell="D451" sqref="D451"/>
+      <selection activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -6190,82 +6190,88 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B465" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C465" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
P00110, P09020, P09030, P09060, S90000, S90001, S90002, S90003, S90004, S90005, S90010, S90011, S90012, S91028, S9308
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E112A3-AD9C-47BF-8F3A-CBE0847A8AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BEF6FC-54E6-4F86-9AF6-34F44475A1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="8745" windowWidth="53205" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="6135" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection activeCell="C470" sqref="C470"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3797,6 +3797,12 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4023,82 +4029,100 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -8940,82 +8964,142 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="1009" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1009" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="1010" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1009" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1009" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="1011" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1010" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1010" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1011" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="1012" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1011" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1011" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1012" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="1013" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1012" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1012" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1013" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="1014" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1013" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1013" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1014" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="1015" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1014" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1014" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1015" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="1016" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1015" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1015" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="1017" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1016" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1016" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1017" t="s">
         <v>1016</v>
       </c>
-    </row>
-    <row r="1018" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1017" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1017" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1018" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="1019" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1018" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1018" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1019" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="1020" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
         <v>1019</v>
       </c>
     </row>
-    <row r="1021" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1021" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="1022" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1022" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1022" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="1023" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1023" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1023" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="1024" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1024" t="s">
         <v>1023</v>
       </c>
@@ -9100,82 +9184,88 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="1041" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1041" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="1042" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1042" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="1043" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1043" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="1044" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1044" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1044" t="s">
         <v>1043</v>
       </c>
     </row>
-    <row r="1045" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1045" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1045" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="1046" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1046" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1046" t="s">
         <v>1045</v>
       </c>
     </row>
-    <row r="1047" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1047" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1047" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="1048" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1048" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1048" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="1049" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1049" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1049" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="1050" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1050" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1050" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="1051" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="1052" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1052" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1052" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="1053" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1053" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1053" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="1054" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1054" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1054" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="1055" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1055" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1055" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="1056" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1055" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1055" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
         <v>1055</v>
       </c>

</xml_diff>

<commit_message>
- S10008, S10009, S10011
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A162B5A1-713D-446B-B37E-9136F17C5F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D80553-2076-4BDC-A7B1-C321029E7981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="7845" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="11820" windowWidth="49560" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3739,7 +3739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="B471" sqref="B471"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <selection activeCell="C474" sqref="C474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -6306,11 +6306,23 @@
       <c r="A473" t="s">
         <v>472</v>
       </c>
+      <c r="B473" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C473" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>473</v>
       </c>
+      <c r="B474" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C474" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
@@ -6320,6 +6332,12 @@
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>475</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C476" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL P00120, S40000, S50000, S50001, S50003, S50004, S93050
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D80553-2076-4BDC-A7B1-C321029E7981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BFD5EA-C806-48BF-B429-2360F8BCAF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="11820" windowWidth="49560" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="16260" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="C474" sqref="C474"/>
+    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="C664" sqref="C664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3808,6 +3808,12 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -7240,82 +7246,88 @@
         <v>655</v>
       </c>
     </row>
-    <row r="657" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="658" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="659" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="660" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="661" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="662" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="663" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="664" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="665" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="666" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="667" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="668" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="669" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="670" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="671" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="672" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B671" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C671" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
         <v>671</v>
       </c>
@@ -7800,82 +7812,106 @@
         <v>767</v>
       </c>
     </row>
-    <row r="769" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="770" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="771" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B770" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C770" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="771" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="772" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B771" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C771" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="772" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="773" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="774" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B773" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C773" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="774" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="775" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B774" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C774" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="775" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="776" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="777" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="778" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="779" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="780" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="781" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="782" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="783" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="784" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
         <v>783</v>
       </c>
@@ -9283,6 +9319,12 @@
     <row r="1053" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1053" t="s">
         <v>1052</v>
+      </c>
+      <c r="B1053" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1053" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="1054" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL P60110, P69020, P69030
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279BA29C-A615-46F3-82EB-EC8290E6BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8769240-A8C1-4941-AE5A-D43F76160B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="15825" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
-      <selection activeCell="B670" sqref="B670"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -5413,82 +5413,88 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B331" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C331" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>335</v>
       </c>
@@ -5573,82 +5579,94 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B365" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B366" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>367</v>
       </c>

</xml_diff>

<commit_message>
TL P32110, P39020, P39030
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8769240-A8C1-4941-AE5A-D43F76160B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0813D516-2D2E-48E5-B6B2-C55FA3992737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="15825" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="B365" sqref="B365"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -4613,82 +4613,88 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -4853,82 +4859,94 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>

</xml_diff>

<commit_message>
TL many scripts (see git log)
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB7013A-20CF-4EB5-8D7E-03112A65A266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95156CF5-8FF9-44EA-A0DA-25ACDC0D236F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="15975" windowWidth="26730" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="18150" windowWidth="55185" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3819,6 +3819,12 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4031,6 +4037,12 @@
       <c r="A45" t="s">
         <v>44</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -4119,6 +4131,12 @@
       <c r="A59" t="s">
         <v>58</v>
       </c>
+      <c r="B59" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -4129,6 +4147,12 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
+      <c r="B61" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -4305,82 +4329,94 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -4465,162 +4501,180 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -4675,6 +4729,12 @@
       <c r="A169" t="s">
         <v>168</v>
       </c>
+      <c r="B169" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
@@ -4711,162 +4771,174 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -5508,11 +5580,23 @@
       <c r="A332" t="s">
         <v>331</v>
       </c>
+      <c r="B332" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C332" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>332</v>
       </c>
+      <c r="B333" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C333" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
@@ -5529,82 +5613,88 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B347" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C347" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>351</v>
       </c>
@@ -5638,11 +5728,23 @@
       <c r="A358" t="s">
         <v>357</v>
       </c>
+      <c r="B358" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C358" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>358</v>
       </c>
+      <c r="B359" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C359" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
@@ -5701,82 +5803,88 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B374" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C374" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>383</v>
       </c>
@@ -5861,82 +5969,88 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B405" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C405" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>415</v>
       </c>
@@ -7929,6 +8043,12 @@
       <c r="A776" t="s">
         <v>775</v>
       </c>
+      <c r="B776" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C776" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
@@ -8464,6 +8584,12 @@
       <c r="A883" t="s">
         <v>882</v>
       </c>
+      <c r="B883" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C883" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
@@ -8794,82 +8920,88 @@
         <v>943</v>
       </c>
     </row>
-    <row r="945" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A945" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="946" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A946" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="947" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A947" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="948" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A948" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="949" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A949" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="950" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A950" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="951" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A951" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="952" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="953" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A953" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="954" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A954" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="955" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="955" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A955" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="956" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="956" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A956" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="957" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B956" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C956" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A957" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="958" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A958" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="959" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A959" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="960" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="960" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A960" t="s">
         <v>959</v>
       </c>
@@ -9254,82 +9386,88 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="1025" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1025" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1025" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="1026" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1026" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1026" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="1027" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1027" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="1028" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1028" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="1029" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1029" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1029" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="1030" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1030" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1030" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="1031" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1031" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1031" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="1032" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1032" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1032" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="1033" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1033" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1033" t="s">
         <v>1032</v>
       </c>
     </row>
-    <row r="1034" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1034" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
         <v>1033</v>
       </c>
     </row>
-    <row r="1035" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1035" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
         <v>1034</v>
       </c>
     </row>
-    <row r="1036" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1036" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1036" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="1037" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1037" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="1038" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1037" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1037" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1038" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="1039" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1039" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1039" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="1040" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1040" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1040" t="s">
         <v>1039</v>
       </c>

</xml_diff>

<commit_message>
TL S50019, S50020, S50025, S70026
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F70719-37F6-4401-AF95-B417DE2983A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D626A6F0-FBFD-4549-BB7B-B150F89930DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="19005" windowWidth="54585" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="19005" windowWidth="54585" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E447" sqref="E447"/>
+    <sheetView tabSelected="1" topLeftCell="A948" workbookViewId="0">
+      <selection activeCell="B961" sqref="B961"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -8117,82 +8117,100 @@
         <v>783</v>
       </c>
     </row>
-    <row r="785" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="786" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="787" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="789" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="790" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B789" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C789" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="791" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B790" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C790" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="791" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="792" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="793" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="794" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="795" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="796" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B795" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C795" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="797" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="798" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="799" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="800" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
         <v>799</v>
       </c>
@@ -9033,82 +9051,88 @@
         <v>959</v>
       </c>
     </row>
-    <row r="961" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="961" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A961" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="962" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B961" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C961" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A962" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="963" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="963" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A963" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="964" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="964" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A964" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="965" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A965" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="966" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A966" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="967" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="967" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A967" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="968" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="968" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A968" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="969" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A969" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="970" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="970" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A970" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="971" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="971" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A971" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="972" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="972" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A972" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="973" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="973" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A973" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="974" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="974" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A974" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="975" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A975" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="976" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A976" t="s">
         <v>975</v>
       </c>

</xml_diff>

<commit_message>
TL S40016, S40027, S40028, S40029, S93020
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D626A6F0-FBFD-4549-BB7B-B150F89930DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57AA946-CD2F-44C9-9B01-1F0588C419D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="19005" windowWidth="54585" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="16320" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A948" workbookViewId="0">
-      <selection activeCell="B961" sqref="B961"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C701" sqref="C701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -7527,162 +7527,186 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="673" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="674" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="675" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="676" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="677" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="678" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="679" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="680" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="681" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="682" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="683" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="684" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="685" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="686" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="687" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="688" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B687" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C687" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="689" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="690" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="691" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="692" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="693" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="694" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="695" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="696" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="697" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="698" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="699" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B698" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C698" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="699" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="700" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B699" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C699" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="701" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B700" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C700" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="702" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="703" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="704" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
         <v>703</v>
       </c>
@@ -9536,6 +9560,12 @@
     <row r="1043" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1043" t="s">
         <v>1042</v>
+      </c>
+      <c r="B1043" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1043" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="1044" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL P01110, P02210, P03110, P09000, P09010
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57AA946-CD2F-44C9-9B01-1F0588C419D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70834B71-3260-4F40-A4A8-59B05B1566EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="16320" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="16065" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C701" sqref="C701"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3850,6 +3850,12 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3881,82 +3887,94 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4073,10 +4091,22 @@
       <c r="A51" t="s">
         <v>50</v>
       </c>
+      <c r="B51" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL S10015, S10016, S10115, S60003
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB452CC3-E89C-488C-BF81-0CE4839C456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B635A5-9E33-4407-AB13-019508EFF3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="16065" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="6240" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="C476" sqref="C476"/>
+    <sheetView tabSelected="1" topLeftCell="A510" workbookViewId="0">
+      <selection activeCell="B527" sqref="B527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -6608,83 +6608,95 @@
       <c r="A480" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B480" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C480" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B481" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>495</v>
       </c>
@@ -6769,82 +6781,88 @@
         <v>511</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B527" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C527" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>527</v>
       </c>
@@ -8801,6 +8819,12 @@
     <row r="896" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
         <v>895</v>
+      </c>
+      <c r="B896" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C896" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="897" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL P00230, P01210, S60004, S60006, S60007, S91029, S91030, S91037
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B635A5-9E33-4407-AB13-019508EFF3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CB95F9-4CAC-4E6F-8B5D-9FCB82B0CD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="6240" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="15780" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A510" workbookViewId="0">
-      <selection activeCell="B527" sqref="B527"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3835,6 +3835,12 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3872,6 +3878,12 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -8827,82 +8839,100 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="897" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="898" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B897" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C897" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="899" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B898" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C898" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="900" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B899" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
         <v>899</v>
       </c>
     </row>
-    <row r="901" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="902" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="903" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="904" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="905" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="906" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="907" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="908" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="909" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="910" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="911" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="912" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
         <v>911</v>
       </c>
@@ -9513,11 +9543,23 @@
       <c r="A1019" t="s">
         <v>1018</v>
       </c>
+      <c r="B1019" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1019" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="1020" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
         <v>1019</v>
       </c>
+      <c r="B1020" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1020" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="1021" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
@@ -9552,6 +9594,12 @@
     <row r="1027" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
         <v>1026</v>
+      </c>
+      <c r="B1027" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1027" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="1028" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add missing old TL files
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CB95F9-4CAC-4E6F-8B5D-9FCB82B0CD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E354E2C3-F93C-4B22-94DF-3030F43B806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="15780" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
+      <selection activeCell="B777" sqref="B777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3889,6 +3889,12 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4016,6 +4022,12 @@
       <c r="A36" t="s">
         <v>35</v>
       </c>
+      <c r="B36" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -4206,11 +4218,23 @@
       <c r="A62" t="s">
         <v>61</v>
       </c>
+      <c r="B62" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
+      <c r="B63" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -4411,6 +4435,12 @@
       <c r="A103" t="s">
         <v>102</v>
       </c>
+      <c r="B103" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
@@ -5017,6 +5047,12 @@
       <c r="A211" t="s">
         <v>210</v>
       </c>
+      <c r="B211" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
@@ -5163,82 +5199,88 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B244" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -5323,82 +5365,94 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -5757,6 +5811,12 @@
       <c r="A353" t="s">
         <v>352</v>
       </c>
+      <c r="B353" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C353" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
@@ -5772,6 +5832,12 @@
       <c r="A356" t="s">
         <v>355</v>
       </c>
+      <c r="B356" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
@@ -8189,6 +8255,12 @@
       <c r="A777" t="s">
         <v>776</v>
       </c>
+      <c r="B777" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C777" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
@@ -9171,6 +9243,12 @@
     <row r="958" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A958" t="s">
         <v>957</v>
+      </c>
+      <c r="B958" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C958" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="959" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL a bunch, see git commit
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E354E2C3-F93C-4B22-94DF-3030F43B806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E747202-CEDE-4D5D-AA14-07E61478A65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="16215" windowWidth="26235" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
-      <selection activeCell="B777" sqref="B777"/>
+    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
+      <selection activeCell="B495" sqref="B495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -6713,41 +6713,89 @@
       <c r="A483" t="s">
         <v>482</v>
       </c>
+      <c r="B483" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>483</v>
       </c>
+      <c r="B484" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>484</v>
       </c>
+      <c r="B485" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>485</v>
       </c>
+      <c r="B486" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C486" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>486</v>
       </c>
+      <c r="B487" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>487</v>
       </c>
+      <c r="B488" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>488</v>
       </c>
+      <c r="B489" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>489</v>
       </c>
+      <c r="B490" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
@@ -6758,15 +6806,33 @@
       <c r="A492" t="s">
         <v>491</v>
       </c>
+      <c r="B492" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C492" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>492</v>
       </c>
+      <c r="B493" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C493" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>493</v>
+      </c>
+      <c r="B494" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C494" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL a bunch (see git commit)
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E747202-CEDE-4D5D-AA14-07E61478A65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16802EEE-B20E-4720-AD01-C6849DAD75BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="16215" windowWidth="26235" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="3510" windowWidth="55245" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
-      <selection activeCell="B495" sqref="B495"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3905,6 +3905,12 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3957,6 +3963,12 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4654,6 +4666,12 @@
       <c r="A142" t="s">
         <v>141</v>
       </c>
+      <c r="B142" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
@@ -4664,6 +4682,12 @@
       <c r="A144" t="s">
         <v>143</v>
       </c>
+      <c r="B144" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
@@ -4818,11 +4842,23 @@
       <c r="A170" t="s">
         <v>169</v>
       </c>
+      <c r="B170" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
+      <c r="B171" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
@@ -5119,82 +5155,88 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -6845,82 +6887,88 @@
         <v>495</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B499" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C499" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>511</v>
       </c>
@@ -9862,11 +9910,23 @@
       <c r="A1048" t="s">
         <v>1047</v>
       </c>
+      <c r="B1048" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1048" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="1049" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1049" t="s">
         <v>1048</v>
       </c>
+      <c r="B1049" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1049" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="1050" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1050" t="s">
@@ -9913,6 +9973,12 @@
     <row r="1056" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
         <v>1055</v>
+      </c>
+      <c r="B1056" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1056" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="1057" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL (see git commit)
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118ECCA8-F030-4632-9D5D-E08B9FA26D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C52501-0675-4959-B937-C7309B5A075C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="6240" windowWidth="55215" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="16710" windowWidth="55215" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3749,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
-      <selection activeCell="A337" sqref="A337"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1045" sqref="B1045"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -4276,6 +4276,12 @@
       <c r="A64" t="s">
         <v>63</v>
       </c>
+      <c r="B64" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -4398,6 +4404,12 @@
       <c r="A86" t="s">
         <v>85</v>
       </c>
+      <c r="B86" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -4860,6 +4872,12 @@
       <c r="A164" t="s">
         <v>163</v>
       </c>
+      <c r="B164" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
@@ -5625,6 +5643,12 @@
       <c r="A293" t="s">
         <v>292</v>
       </c>
+      <c r="B293" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
@@ -5904,6 +5928,12 @@
       <c r="A338" t="s">
         <v>337</v>
       </c>
+      <c r="B338" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C338" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
@@ -7257,82 +7287,88 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B529" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C529" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>543</v>
       </c>
@@ -10092,6 +10128,12 @@
     <row r="1045" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1045" t="s">
         <v>1044</v>
+      </c>
+      <c r="B1045" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C1045" s="3" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="1046" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TL ( see git commit)
</commit_message>
<xml_diff>
--- a/tl/progress.xlsx
+++ b/tl/progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C52501-0675-4959-B937-C7309B5A075C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCD8AEA-8538-4FCD-8F42-78E2197F63CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="16710" windowWidth="55215" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="4680" windowWidth="55215" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00101.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="1112">
   <si>
     <t>Edited</t>
   </si>
@@ -3750,7 +3750,7 @@
   <dimension ref="A1:E1108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1045" sqref="B1045"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,11 +3782,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <f>COUNTA(B3:B1108)</f>
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTA(C3:C1108)</f>
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D2" s="3">
         <f>COUNTA(D3:D1108)</f>
@@ -3846,6 +3846,12 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4002,6 +4008,12 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
+      <c r="B26" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -4069,6 +4081,12 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
+      <c r="B37" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -4116,6 +4134,12 @@
       <c r="A44" t="s">
         <v>43</v>
       </c>
+      <c r="B44" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -4287,6 +4311,12 @@
       <c r="A65" t="s">
         <v>64</v>
       </c>
+      <c r="B65" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -4565,82 +4595,88 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -4795,6 +4831,12 @@
       <c r="A151" t="s">
         <v>150</v>
       </c>
+      <c r="B151" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -5587,6 +5629,12 @@
       <c r="A283" t="s">
         <v>282</v>
       </c>
+      <c r="B283" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
@@ -5597,6 +5645,12 @@
       <c r="A285" t="s">
         <v>284</v>
       </c>
+      <c r="B285" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
@@ -5674,6 +5728,12 @@
       <c r="A298" t="s">
         <v>297</v>
       </c>
+      <c r="B298" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
@@ -5939,6 +5999,12 @@
       <c r="A339" t="s">
         <v>338</v>
       </c>
+      <c r="B339" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
@@ -6037,6 +6103,12 @@
       <c r="A355" t="s">
         <v>354</v>
       </c>
+      <c r="B355" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
@@ -7373,82 +7445,94 @@
         <v>543</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B547" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C547" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B548" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C548" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>559</v>
       </c>

</xml_diff>